<commit_message>
Almost Done with the Base Table
</commit_message>
<xml_diff>
--- a/Copy of Fake News List and Claim.xlsx
+++ b/Copy of Fake News List and Claim.xlsx
@@ -4852,8 +4852,8 @@
   </sheetPr>
   <dimension ref="A1:C999"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A6" sqref="A6"/>
+    <sheetView tabSelected="1" topLeftCell="A28" workbookViewId="0">
+      <selection activeCell="A50" sqref="A50"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -5059,7 +5059,7 @@
       </c>
       <c r="B20" s="6"/>
     </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:3" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A21" s="7" t="s">
         <v>181</v>
       </c>
@@ -5070,7 +5070,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:3" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A22" s="7" t="s">
         <v>190</v>
       </c>
@@ -5081,7 +5081,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:3" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A23" s="7" t="s">
         <v>195</v>
       </c>
@@ -5092,7 +5092,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:3" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A24" s="7" t="s">
         <v>198</v>
       </c>
@@ -5103,7 +5103,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:3" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A25" s="7" t="s">
         <v>201</v>
       </c>
@@ -5114,7 +5114,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:3" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A26" s="7" t="s">
         <v>207</v>
       </c>
@@ -5125,7 +5125,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:3" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A27" s="7" t="s">
         <v>211</v>
       </c>
@@ -5289,6 +5289,9 @@
       </c>
     </row>
     <row r="42" spans="1:3" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="A42" s="1" t="s">
+        <v>278</v>
+      </c>
       <c r="B42" s="6"/>
     </row>
     <row r="43" spans="1:3" ht="13.2" x14ac:dyDescent="0.25">
@@ -5304,9 +5307,6 @@
       <c r="B46" s="6"/>
     </row>
     <row r="47" spans="1:3" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A47" s="1" t="s">
-        <v>278</v>
-      </c>
       <c r="B47" s="6"/>
     </row>
     <row r="48" spans="1:3" ht="13.2" x14ac:dyDescent="0.25">
@@ -8219,7 +8219,7 @@
   </sheetPr>
   <dimension ref="A1:F834"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="A803" workbookViewId="0">
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
@@ -17960,10 +17960,10 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:C333"/>
+  <dimension ref="A1:C329"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+    <sheetView topLeftCell="A319" workbookViewId="0">
+      <selection activeCell="A335" sqref="A335"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -21581,8 +21581,8 @@
         <v>210</v>
       </c>
     </row>
-    <row r="333" spans="1:3" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A333" s="2" t="s">
+    <row r="329" spans="1:3" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="A329" s="2" t="s">
         <v>840</v>
       </c>
     </row>
@@ -21901,7 +21901,7 @@
     <hyperlink ref="A326" r:id="rId311"/>
     <hyperlink ref="A327" r:id="rId312"/>
     <hyperlink ref="A328" r:id="rId313"/>
-    <hyperlink ref="A333" r:id="rId314"/>
+    <hyperlink ref="A329" r:id="rId314"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Add more trustworthy sites
</commit_message>
<xml_diff>
--- a/Copy of Fake News List and Claim.xlsx
+++ b/Copy of Fake News List and Claim.xlsx
@@ -62,7 +62,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3433" uniqueCount="1471">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3447" uniqueCount="1485">
   <si>
     <t>type</t>
   </si>
@@ -4475,6 +4475,48 @@
   </si>
   <si>
     <t>bbc.com</t>
+  </si>
+  <si>
+    <t>nytimes.com</t>
+  </si>
+  <si>
+    <t>wsj.com</t>
+  </si>
+  <si>
+    <t>theguardian.com</t>
+  </si>
+  <si>
+    <t>cnn.com</t>
+  </si>
+  <si>
+    <t>foxnews.com</t>
+  </si>
+  <si>
+    <t>aljazeera.com</t>
+  </si>
+  <si>
+    <t>washingtonpost.com</t>
+  </si>
+  <si>
+    <t>reuters.com</t>
+  </si>
+  <si>
+    <t>economist.com</t>
+  </si>
+  <si>
+    <t>ap.org</t>
+  </si>
+  <si>
+    <t>c-span.org</t>
+  </si>
+  <si>
+    <t>pbs.org</t>
+  </si>
+  <si>
+    <t>npr.org</t>
+  </si>
+  <si>
+    <t>reut.rs</t>
   </si>
 </sst>
 </file>
@@ -4855,8 +4897,8 @@
   </sheetPr>
   <dimension ref="A1:C999"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
-      <selection activeCell="A44" sqref="A44"/>
+    <sheetView tabSelected="1" topLeftCell="A34" workbookViewId="0">
+      <selection activeCell="A57" sqref="A57"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.453125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -5304,66 +5346,108 @@
       <c r="B43" s="6"/>
     </row>
     <row r="44" spans="1:3" ht="12.5" x14ac:dyDescent="0.25">
+      <c r="A44" t="s">
+        <v>1471</v>
+      </c>
       <c r="B44" s="6"/>
     </row>
     <row r="45" spans="1:3" ht="12.5" x14ac:dyDescent="0.25">
+      <c r="A45" t="s">
+        <v>1472</v>
+      </c>
       <c r="B45" s="6"/>
     </row>
     <row r="46" spans="1:3" ht="12.5" x14ac:dyDescent="0.25">
+      <c r="A46" t="s">
+        <v>1473</v>
+      </c>
       <c r="B46" s="6"/>
     </row>
     <row r="47" spans="1:3" ht="12.5" x14ac:dyDescent="0.25">
+      <c r="A47" t="s">
+        <v>1474</v>
+      </c>
       <c r="B47" s="6"/>
     </row>
     <row r="48" spans="1:3" ht="12.5" x14ac:dyDescent="0.25">
+      <c r="A48" t="s">
+        <v>1475</v>
+      </c>
       <c r="B48" s="6"/>
     </row>
-    <row r="49" spans="2:2" ht="12.5" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:2" ht="12.5" x14ac:dyDescent="0.25">
+      <c r="A49" t="s">
+        <v>1476</v>
+      </c>
       <c r="B49" s="6"/>
     </row>
-    <row r="50" spans="2:2" ht="12.5" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:2" ht="12.5" x14ac:dyDescent="0.25">
+      <c r="A50" t="s">
+        <v>1477</v>
+      </c>
       <c r="B50" s="6"/>
     </row>
-    <row r="51" spans="2:2" ht="12.5" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:2" ht="12.5" x14ac:dyDescent="0.25">
+      <c r="A51" t="s">
+        <v>1478</v>
+      </c>
       <c r="B51" s="6"/>
     </row>
-    <row r="52" spans="2:2" ht="12.5" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:2" ht="12.5" x14ac:dyDescent="0.25">
+      <c r="A52" t="s">
+        <v>1479</v>
+      </c>
       <c r="B52" s="6"/>
     </row>
-    <row r="53" spans="2:2" ht="12.5" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:2" ht="12.5" x14ac:dyDescent="0.25">
+      <c r="A53" t="s">
+        <v>1480</v>
+      </c>
       <c r="B53" s="6"/>
     </row>
-    <row r="54" spans="2:2" ht="12.5" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:2" ht="12.5" x14ac:dyDescent="0.25">
+      <c r="A54" t="s">
+        <v>1481</v>
+      </c>
       <c r="B54" s="6"/>
     </row>
-    <row r="55" spans="2:2" ht="12.5" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:2" ht="12.5" x14ac:dyDescent="0.25">
+      <c r="A55" t="s">
+        <v>1482</v>
+      </c>
       <c r="B55" s="6"/>
     </row>
-    <row r="56" spans="2:2" ht="12.5" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:2" ht="12.5" x14ac:dyDescent="0.25">
+      <c r="A56" t="s">
+        <v>1483</v>
+      </c>
       <c r="B56" s="6"/>
     </row>
-    <row r="57" spans="2:2" ht="12.5" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:2" ht="12.5" x14ac:dyDescent="0.25">
+      <c r="A57" t="s">
+        <v>1484</v>
+      </c>
       <c r="B57" s="6"/>
     </row>
-    <row r="58" spans="2:2" ht="12.5" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:2" ht="12.5" x14ac:dyDescent="0.25">
       <c r="B58" s="6"/>
     </row>
-    <row r="59" spans="2:2" ht="12.5" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:2" ht="12.5" x14ac:dyDescent="0.25">
       <c r="B59" s="6"/>
     </row>
-    <row r="60" spans="2:2" ht="12.5" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:2" ht="12.5" x14ac:dyDescent="0.25">
       <c r="B60" s="6"/>
     </row>
-    <row r="61" spans="2:2" ht="12.5" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:2" ht="12.5" x14ac:dyDescent="0.25">
       <c r="B61" s="6"/>
     </row>
-    <row r="62" spans="2:2" ht="12.5" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:2" ht="12.5" x14ac:dyDescent="0.25">
       <c r="B62" s="6"/>
     </row>
-    <row r="63" spans="2:2" ht="12.5" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:2" ht="12.5" x14ac:dyDescent="0.25">
       <c r="B63" s="6"/>
     </row>
-    <row r="64" spans="2:2" ht="12.5" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:2" ht="12.5" x14ac:dyDescent="0.25">
       <c r="B64" s="6"/>
     </row>
     <row r="65" spans="2:2" ht="12.5" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
added a few more sources of news
</commit_message>
<xml_diff>
--- a/Copy of Fake News List and Claim.xlsx
+++ b/Copy of Fake News List and Claim.xlsx
@@ -62,7 +62,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3448" uniqueCount="1486">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3449" uniqueCount="1487">
   <si>
     <t>type</t>
   </si>
@@ -4520,6 +4520,9 @@
   </si>
   <si>
     <t>www.businessinsider.com</t>
+  </si>
+  <si>
+    <t>Forbes.com</t>
   </si>
 </sst>
 </file>
@@ -4900,8 +4903,8 @@
   </sheetPr>
   <dimension ref="A1:C999"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A34" workbookViewId="0">
-      <selection activeCell="A59" sqref="A59"/>
+    <sheetView tabSelected="1" topLeftCell="A40" workbookViewId="0">
+      <selection activeCell="A64" sqref="A64"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -5439,6 +5442,9 @@
       <c r="B58" s="6"/>
     </row>
     <row r="59" spans="1:2" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="A59" t="s">
+        <v>1486</v>
+      </c>
       <c r="B59" s="6"/>
     </row>
     <row r="60" spans="1:2" ht="13.2" x14ac:dyDescent="0.25">
@@ -8315,7 +8321,7 @@
   </sheetPr>
   <dimension ref="A1:F834"/>
   <sheetViews>
-    <sheetView topLeftCell="A523" workbookViewId="0">
+    <sheetView topLeftCell="A565" workbookViewId="0">
       <selection activeCell="A518" sqref="A518"/>
     </sheetView>
   </sheetViews>

</xml_diff>